<commit_message>
revised version after a discussion with Mathias
</commit_message>
<xml_diff>
--- a/Interactive Maps- MARG.xlsx
+++ b/Interactive Maps- MARG.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="399">
   <si>
     <t>Entries ID</t>
   </si>
@@ -358,6 +358,9 @@
     <t>UMR MARBEC, France</t>
   </si>
   <si>
+    <t>-20.233792, 57.497536</t>
+  </si>
+  <si>
     <t>hsalencia@gmail.com</t>
   </si>
   <si>
@@ -403,6 +406,9 @@
     <t>Vrije Universiteit Brussel</t>
   </si>
   <si>
+    <t>-6.783409, 39.202595</t>
+  </si>
+  <si>
     <t>gofaka@gmail.com</t>
   </si>
   <si>
@@ -478,6 +484,9 @@
     <t>KENYA MARINE AND FISHERIES RESEARCH INSTITUTE</t>
   </si>
   <si>
+    <t>-4.055072, 39.682070</t>
+  </si>
+  <si>
     <t>Inter-annual trophic plasticity of seagrass-associated fishes in the context of artisanal overfishing (SW Madagascar)</t>
   </si>
   <si>
@@ -796,6 +805,9 @@
     <t>University of Florida -School of Natural Resources and Environment</t>
   </si>
   <si>
+    <t>-2.292321, 40.866876</t>
+  </si>
+  <si>
     <t>nwambiji@gmail.com</t>
   </si>
   <si>
@@ -1114,18 +1126,6 @@
     <t>Dr. Michelle Caputo Caputo</t>
   </si>
   <si>
-    <t>Mr. Benjamini Lupinga</t>
-  </si>
-  <si>
-    <t>The Asian and African Reconciliation on Law</t>
-  </si>
-  <si>
-    <t>Tanzania Law Society</t>
-  </si>
-  <si>
-    <t>-6.810853, 39.292217</t>
-  </si>
-  <si>
     <t>-23.352314, 43.666683</t>
   </si>
   <si>
@@ -1144,9 +1144,6 @@
     <t>-6.158101, 39.192197</t>
   </si>
   <si>
-    <t>-4.055072, 39.682070</t>
-  </si>
-  <si>
     <t>-23.855772, 35.548924</t>
   </si>
   <si>
@@ -1198,9 +1195,6 @@
     <t>-33.957627, 18.461129</t>
   </si>
   <si>
-    <t>-6.783409, 39.202595</t>
-  </si>
-  <si>
     <t>UNIVERSITY OF DODOMA</t>
   </si>
   <si>
@@ -1214,9 +1208,6 @@
   </si>
   <si>
     <t>-29.867406, 30.980699</t>
-  </si>
-  <si>
-    <t>-20.233792, 57.497536</t>
   </si>
   <si>
     <t>-33.933493, 18.627962</t>
@@ -1233,10 +1224,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -1310,29 +1301,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1353,25 +1329,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="0"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1393,24 +1360,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1425,7 +1376,62 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1439,22 +1445,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1499,19 +1490,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1529,7 +1520,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1541,7 +1544,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1553,7 +1592,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1565,121 +1664,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1801,6 +1792,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1812,24 +1812,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1856,15 +1838,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1898,151 +1871,169 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="11" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2383,8 +2374,8 @@
   </sheetPr>
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15.75" customHeight="1"/>
@@ -3360,9 +3351,8 @@
       <c r="I28" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="J28" s="3" t="str">
-        <f>VLOOKUP(I28,Locations!$B$2:$C$78,2,0)</f>
-        <v>43.557031, 3.918829</v>
+      <c r="J28" s="3" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="29" ht="14.4" spans="1:10">
@@ -3376,13 +3366,13 @@
         <v>12</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>55</v>
@@ -3409,22 +3399,22 @@
         <v>12</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>22</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J30" s="3" t="str">
         <f>VLOOKUP(I30,Locations!$B$2:$C$78,2,0)</f>
@@ -3442,13 +3432,13 @@
         <v>12</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>16</v>
@@ -3475,13 +3465,13 @@
         <v>12</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>16</v>
@@ -3490,11 +3480,10 @@
         <v>17</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="J32" s="3" t="str">
-        <f>VLOOKUP(I32,Locations!$B$2:$C$78,2,0)</f>
-        <v>50.822983, 4.392628</v>
+        <v>127</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="33" ht="14.4" spans="1:10">
@@ -3508,13 +3497,13 @@
         <v>12</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>16</v>
@@ -3541,13 +3530,13 @@
         <v>12</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>16</v>
@@ -3574,13 +3563,13 @@
         <v>12</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>16</v>
@@ -3589,7 +3578,7 @@
         <v>17</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="J35" s="3" t="str">
         <f>VLOOKUP(I35,Locations!$B$2:$C$78,2,0)</f>
@@ -3607,13 +3596,13 @@
         <v>12</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>16</v>
@@ -3646,7 +3635,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:L9"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15.75" customHeight="1"/>
@@ -3681,10 +3670,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="K1" s="15" t="s">
         <v>9</v>
@@ -3704,28 +3693,28 @@
         <v>2019</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>55</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>56</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="K2" s="3" t="str">
         <f>VLOOKUP(I2,Locations!$B$2:$C$78,2,0)</f>
@@ -3741,32 +3730,31 @@
         <v>2019</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>36</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="K3" s="3" t="str">
-        <f>VLOOKUP(I3,Locations!$B$2:$C$78,2,0)</f>
-        <v>-4.055072, 39.682070</v>
+        <v>153</v>
+      </c>
+      <c r="K3" t="s">
+        <v>154</v>
       </c>
       <c r="L3" s="3"/>
     </row>
@@ -3778,7 +3766,7 @@
         <v>2019</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D4" s="20" t="s">
         <v>45</v>
@@ -3787,19 +3775,19 @@
         <v>46</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="G4" s="20" t="s">
         <v>27</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="K4" s="3" t="str">
         <f>VLOOKUP(I4,Locations!$B$2:$C$78,2,0)</f>
@@ -3815,28 +3803,28 @@
         <v>2019</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="G5" s="20" t="s">
         <v>36</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="K5" s="3" t="str">
         <f>VLOOKUP(I5,Locations!$B$2:$C$78,2,0)</f>
@@ -3852,28 +3840,28 @@
         <v>2019</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>23</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="K6" s="3" t="str">
         <f>VLOOKUP(I6,Locations!$B$2:$C$78,2,0)</f>
@@ -3889,28 +3877,28 @@
         <v>2019</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="K7" s="3" t="str">
         <f>VLOOKUP(I7,Locations!$B$2:$C$78,2,0)</f>
@@ -3926,28 +3914,28 @@
         <v>2019</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>51</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="K8" s="3" t="str">
         <f>VLOOKUP(I8,Locations!$B$2:$C$78,2,0)</f>
@@ -3963,28 +3951,28 @@
         <v>2019</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="K9" s="3" t="str">
         <f>VLOOKUP(I9,Locations!$B$2:$C$78,2,0)</f>
@@ -4000,28 +3988,28 @@
         <v>2018</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="K10" s="3" t="str">
         <f>VLOOKUP(I10,Locations!$B$2:$C$78,2,0)</f>
@@ -4037,28 +4025,28 @@
         <v>2018</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>69</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="K11" s="3" t="str">
         <f>VLOOKUP(I11,Locations!$B$2:$C$78,2,0)</f>
@@ -4074,28 +4062,28 @@
         <v>2018</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>27</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="K12" s="3" t="str">
         <f>VLOOKUP(I12,Locations!$B$2:$C$78,2,0)</f>
@@ -4111,28 +4099,28 @@
         <v>2018</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>36</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="K13" s="3" t="str">
         <f>VLOOKUP(I13,Locations!$B$2:$C$78,2,0)</f>
@@ -4148,28 +4136,28 @@
         <v>2018</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>16</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>69</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="K14" s="3" t="str">
         <f>VLOOKUP(I14,Locations!$B$2:$C$78,2,0)</f>
@@ -4185,28 +4173,28 @@
         <v>2018</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>110</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="K15" s="3" t="str">
         <f>VLOOKUP(I15,Locations!$B$2:$C$78,2,0)</f>
@@ -4222,28 +4210,28 @@
         <v>2018</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="G16" s="20" t="s">
         <v>16</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>51</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="K16" s="3" t="str">
         <f>VLOOKUP(I16,Locations!$B$2:$C$78,2,0)</f>
@@ -4265,10 +4253,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:M46"/>
+  <dimension ref="A2:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E17" workbookViewId="0">
-      <selection activeCell="L43" sqref="L43"/>
+    <sheetView tabSelected="1" topLeftCell="E36" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15.75" customHeight="1"/>
@@ -4296,7 +4284,7 @@
         <v>4</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>6</v>
@@ -4305,10 +4293,10 @@
         <v>7</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="K2" s="13" t="s">
         <v>9</v>
@@ -4328,28 +4316,28 @@
         <v>2018</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>36</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="K3" s="3" t="str">
         <f>VLOOKUP(J3,Locations!$B$2:$C$78,2,0)</f>
@@ -4366,28 +4354,28 @@
         <v>2018</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>110</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="K4" s="3" t="str">
         <f>VLOOKUP(J4,Locations!$B$2:$C$78,2,0)</f>
@@ -4404,28 +4392,28 @@
         <v>2018</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>110</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="K5" s="3" t="str">
         <f>VLOOKUP(J5,Locations!$B$2:$C$78,2,0)</f>
@@ -4442,28 +4430,28 @@
         <v>2018</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="K6" s="3" t="str">
         <f>VLOOKUP(J6,Locations!$B$2:$C$78,2,0)</f>
@@ -4480,28 +4468,28 @@
         <v>2018</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="K7" s="3" t="str">
         <f>VLOOKUP(J7,Locations!$B$2:$C$78,2,0)</f>
@@ -4518,25 +4506,25 @@
         <v>2018</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>23</v>
@@ -4556,25 +4544,25 @@
         <v>2018</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>36</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>37</v>
@@ -4594,28 +4582,28 @@
         <v>2018</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>36</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="K10" s="3" t="str">
         <f>VLOOKUP(J10,Locations!$B$2:$C$78,2,0)</f>
@@ -4632,28 +4620,28 @@
         <v>2018</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="K11" s="3" t="str">
         <f>VLOOKUP(J11,Locations!$B$2:$C$78,2,0)</f>
@@ -4670,25 +4658,25 @@
         <v>2018</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>55</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>56</v>
@@ -4708,32 +4696,31 @@
         <v>2018</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>36</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="K13" s="3" t="str">
-        <f>VLOOKUP(J13,Locations!$B$2:$C$78,2,0)</f>
-        <v>29.643792, -82.354846</v>
+        <v>260</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>261</v>
       </c>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
@@ -4746,25 +4733,25 @@
         <v>2018</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="E14" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>259</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>256</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>36</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>37</v>
@@ -4784,28 +4771,28 @@
         <v>2018</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="K15" s="3" t="str">
         <f>VLOOKUP(J15,Locations!$B$2:$C$78,2,0)</f>
@@ -4822,25 +4809,25 @@
         <v>2018</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>36</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>37</v>
@@ -4860,25 +4847,25 @@
         <v>2018</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>27</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>28</v>
@@ -4898,28 +4885,28 @@
         <v>2018</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="K18" s="3" t="str">
         <f>VLOOKUP(J18,Locations!$B$2:$C$78,2,0)</f>
@@ -4936,25 +4923,25 @@
         <v>2018</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>36</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>37</v>
@@ -4974,28 +4961,28 @@
         <v>2018</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>36</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="K20" s="3" t="str">
         <f>VLOOKUP(J20,Locations!$B$2:$C$78,2,0)</f>
@@ -5012,25 +4999,25 @@
         <v>2018</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>69</v>
@@ -5050,22 +5037,22 @@
         <v>2018</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>27</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I22" s="3"/>
       <c r="J22" s="3" t="s">
@@ -5086,22 +5073,22 @@
         <v>2018</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>27</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3" t="s">
@@ -5122,22 +5109,22 @@
         <v>2018</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="3" t="s">
@@ -5158,26 +5145,26 @@
         <v>2018</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>36</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I25" s="3"/>
       <c r="J25" s="3" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="K25" s="3" t="str">
         <f>VLOOKUP(J25,Locations!$B$2:$C$78,2,0)</f>
@@ -5194,26 +5181,26 @@
         <v>2018</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I26" s="3"/>
       <c r="J26" s="3" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="K26" s="3" t="str">
         <f>VLOOKUP(J26,Locations!$B$2:$C$78,2,0)</f>
@@ -5230,26 +5217,26 @@
         <v>2018</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="3" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="K27" s="3" t="str">
         <f>VLOOKUP(J27,Locations!$B$2:$C$78,2,0)</f>
@@ -5266,26 +5253,26 @@
         <v>2018</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="E28" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>302</v>
-      </c>
       <c r="G28" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="3" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="K28" s="3" t="str">
         <f>VLOOKUP(J28,Locations!$B$2:$C$78,2,0)</f>
@@ -5302,26 +5289,26 @@
         <v>2018</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I29" s="3"/>
       <c r="J29" s="3" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="K29" s="3" t="str">
         <f>VLOOKUP(J29,Locations!$B$2:$C$78,2,0)</f>
@@ -5338,26 +5325,26 @@
         <v>2019</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I30" s="3"/>
       <c r="J30" s="3" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="K30" s="3" t="str">
         <f>VLOOKUP(J30,Locations!$B$2:$C$78,2,0)</f>
@@ -5374,26 +5361,26 @@
         <v>2019</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I31" s="3"/>
       <c r="J31" s="3" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="K31" s="3" t="str">
         <f>VLOOKUP(J31,Locations!$B$2:$C$78,2,0)</f>
@@ -5410,22 +5397,22 @@
         <v>2019</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I32" s="3"/>
       <c r="J32" s="3" t="s">
@@ -5446,26 +5433,26 @@
         <v>2019</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I33" s="3"/>
       <c r="J33" s="3" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="K33" s="3" t="str">
         <f>VLOOKUP(J33,Locations!$B$2:$C$78,2,0)</f>
@@ -5482,22 +5469,22 @@
         <v>2019</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>104</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I34" s="3"/>
       <c r="J34" s="3" t="s">
@@ -5518,26 +5505,26 @@
         <v>2019</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I35" s="3"/>
       <c r="J35" s="3" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="K35" s="3" t="str">
         <f>VLOOKUP(J35,Locations!$B$2:$C$78,2,0)</f>
@@ -5554,26 +5541,26 @@
         <v>2019</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I36" s="3"/>
       <c r="J36" s="3" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="K36" s="3" t="str">
         <f>VLOOKUP(J36,Locations!$B$2:$C$78,2,0)</f>
@@ -5590,26 +5577,26 @@
         <v>2019</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I37" s="3"/>
       <c r="J37" s="3" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="K37" s="3" t="str">
         <f>VLOOKUP(J37,Locations!$B$2:$C$78,2,0)</f>
@@ -5626,26 +5613,26 @@
         <v>2019</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I38" s="3"/>
       <c r="J38" s="3" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="K38" s="3" t="str">
         <f>VLOOKUP(J38,Locations!$B$2:$C$78,2,0)</f>
@@ -5662,26 +5649,26 @@
         <v>2019</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I39" s="3"/>
       <c r="J39" s="3" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="K39" s="3" t="str">
         <f>VLOOKUP(J39,Locations!$B$2:$C$78,2,0)</f>
@@ -5698,26 +5685,26 @@
         <v>2019</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I40" s="3"/>
       <c r="J40" s="3" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="K40" s="3" t="str">
         <f>VLOOKUP(J40,Locations!$B$2:$C$78,2,0)</f>
@@ -5734,26 +5721,26 @@
         <v>2019</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="K41" s="3" t="str">
         <f>VLOOKUP(J41,Locations!$B$2:$C$78,2,0)</f>
@@ -5770,26 +5757,26 @@
         <v>2019</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I42" s="3"/>
       <c r="J42" s="3" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="K42" s="3" t="str">
         <f>VLOOKUP(J42,Locations!$B$2:$C$78,2,0)</f>
@@ -5806,26 +5793,26 @@
         <v>2019</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I43" s="3"/>
       <c r="J43" s="3" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="K43" s="3" t="str">
         <f>VLOOKUP(J43,Locations!$B$2:$C$78,2,0)</f>
@@ -5842,26 +5829,26 @@
         <v>2019</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I44" s="3"/>
       <c r="J44" s="3" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="K44" s="3" t="str">
         <f>VLOOKUP(J44,Locations!$B$2:$C$78,2,0)</f>
@@ -5878,26 +5865,26 @@
         <v>2019</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I45" s="3"/>
       <c r="J45" s="3" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="K45" s="3" t="str">
         <f>VLOOKUP(J45,Locations!$B$2:$C$78,2,0)</f>
@@ -5905,32 +5892,6 @@
       </c>
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
-    </row>
-    <row r="46" customHeight="1" spans="2:11">
-      <c r="B46">
-        <v>2019</v>
-      </c>
-      <c r="C46" t="s">
-        <v>209</v>
-      </c>
-      <c r="E46" t="s">
-        <v>364</v>
-      </c>
-      <c r="F46" t="s">
-        <v>365</v>
-      </c>
-      <c r="G46" t="s">
-        <v>323</v>
-      </c>
-      <c r="H46" t="s">
-        <v>146</v>
-      </c>
-      <c r="J46" t="s">
-        <v>366</v>
-      </c>
-      <c r="K46" t="s">
-        <v>367</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5959,7 +5920,7 @@
     <row r="1" ht="14.4" spans="1:3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>9</v>
@@ -5977,7 +5938,7 @@
     <row r="3" ht="14.4" spans="1:3">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>369</v>
@@ -5995,7 +5956,7 @@
     <row r="5" ht="14.4" spans="1:3">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>371</v>
@@ -6025,25 +5986,25 @@
         <v>37</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>374</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" ht="14.4" spans="1:3">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="10" ht="14.4" spans="1:3">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="11" ht="14.4" spans="1:3">
@@ -6052,25 +6013,25 @@
         <v>44</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="12" ht="14.4" spans="1:3">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="13" ht="14.4" spans="1:3">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="14" ht="14.4" spans="1:3">
@@ -6079,85 +6040,85 @@
         <v>85</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="15" ht="14.4" spans="1:3">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="16" ht="14.4" spans="1:3">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="17" ht="14.4" spans="1:3">
       <c r="A17" s="8"/>
       <c r="B17" s="3" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="18" ht="14.4" spans="1:3">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="19" ht="14.4" spans="1:3">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="20" ht="14.4" spans="1:3">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="21" ht="14.4" spans="2:3">
       <c r="B21" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="22" ht="14.4" spans="2:3">
       <c r="B22" s="3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="23" ht="14.4" spans="2:3">
       <c r="B23" s="3" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="24" ht="13.2" spans="2:3">
@@ -6165,15 +6126,15 @@
         <v>51</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="25" ht="14.4" spans="2:3">
       <c r="B25" s="3" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="26" ht="14.4" spans="2:3">
@@ -6181,15 +6142,15 @@
         <v>111</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="27" ht="14.4" spans="2:3">
       <c r="B27" s="3" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="28" ht="14.4" spans="2:3">
@@ -6197,68 +6158,68 @@
         <v>23</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>392</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" ht="14.4" spans="2:3">
       <c r="B29" s="3" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="30" ht="14.4" spans="2:3">
       <c r="B30" s="3" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="31" ht="14.4" spans="2:3">
       <c r="B31" s="3" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="32" ht="14.4" spans="2:3">
       <c r="B32" s="3" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="33" ht="14.4" spans="2:3">
       <c r="B33" s="11" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>398</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" ht="14.4" spans="2:3">
       <c r="B34" s="12" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="35" ht="14.4" spans="2:3">
       <c r="B35" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="36" ht="14.4" spans="2:3">
       <c r="B36" s="3" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>369</v>
@@ -6266,7 +6227,7 @@
     </row>
     <row r="37" ht="14.4" spans="2:3">
       <c r="B37" s="3" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>373</v>
@@ -6274,7 +6235,7 @@
     </row>
     <row r="38" ht="14.4" spans="2:3">
       <c r="B38" s="3" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>373</v>

</xml_diff>

<commit_message>
push the revised version
</commit_message>
<xml_diff>
--- a/Interactive Maps- MARG.xlsx
+++ b/Interactive Maps- MARG.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9264" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="9264"/>
   </bookViews>
   <sheets>
     <sheet name="MARG I" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
     <t>Dr. Blandina Robert LUGENDO</t>
   </si>
   <si>
-    <t>THE POTENTIAL ROLE OF MANGROVES IN PROTECTING ADJACENT MARINE HABITATS FROM LAND-DERIVED NUTRIENT LOADS</t>
+    <t>The potential role of mangroves in protecting adjacent marine habitats from land-derived nutrient loads</t>
   </si>
   <si>
     <t>F</t>
@@ -910,7 +910,7 @@
     <t>Ms Marcelina Felix Mushi</t>
   </si>
   <si>
-    <t>Sao Paulo School Of Advanced Science On Ocean Interdisciplinary Research Andgovernance.</t>
+    <t>Sao Paulo School Of Advanced Science On Ocean Interdisciplinary Research And governance.</t>
   </si>
   <si>
     <t>editor@theioo.com</t>
@@ -1060,13 +1060,13 @@
     <t>14th Universiti Malaysia Terengganu International Annual Symposium 2019</t>
   </si>
   <si>
+    <t>r.bhagooli@uom.ac.mu</t>
+  </si>
+  <si>
+    <t>Dr. Ranjeet Bhagooli Bhagooli</t>
+  </si>
+  <si>
     <t>Mauritian</t>
-  </si>
-  <si>
-    <t>r.bhagooli@uom.ac.mu</t>
-  </si>
-  <si>
-    <t>Dr. Ranjeet Bhagooli Bhagooli</t>
   </si>
   <si>
     <t>abdulalawiy@ymail.com</t>
@@ -1224,10 +1224,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -1308,7 +1308,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1330,7 +1352,38 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1346,7 +1399,30 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1355,13 +1431,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1376,76 +1445,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1490,25 +1490,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1520,31 +1508,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1562,19 +1526,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1586,7 +1604,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1598,7 +1646,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1610,67 +1664,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1792,11 +1792,50 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1816,17 +1855,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1856,184 +1889,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2374,8 +2374,8 @@
   </sheetPr>
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15.75" customHeight="1"/>
@@ -4255,8 +4255,8 @@
   </sheetPr>
   <dimension ref="A2:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E36" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView topLeftCell="E20" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15.75" customHeight="1"/>
@@ -5625,7 +5625,7 @@
         <v>345</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>346</v>
+        <v>110</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>148</v>
@@ -5652,16 +5652,16 @@
         <v>212</v>
       </c>
       <c r="D39" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="E39" s="3" t="s">
         <v>347</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>348</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>345</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>148</v>
@@ -5733,7 +5733,7 @@
         <v>345</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>148</v>

</xml_diff>